<commit_message>
jegyzokonyv + formazasi valtoztatasok
</commit_message>
<xml_diff>
--- a/JMDRGG_0316/2.feladat.xlsx
+++ b/JMDRGG_0316/2.feladat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://diakoffice-my.sharepoint.com/personal/rob__sulid_hu/Documents/EGYETEM/2020-2021-02/Operacios_rendszerek/gyakorlat/JMDRGGOsGyak/JMDRGG_0316/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{DC6181CA-A301-4551-BD5A-F10134151926}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{40343C31-2BEE-4850-8443-B275FC336F97}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{DC6181CA-A301-4551-BD5A-F10134151926}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A2EA6E96-17CD-476B-B012-BBE0298535A0}"/>
   <bookViews>
-    <workbookView xWindow="6390" yWindow="1005" windowWidth="17280" windowHeight="11385" xr2:uid="{470C459F-9058-417E-8659-1849A433C267}"/>
+    <workbookView xWindow="7875" yWindow="450" windowWidth="17280" windowHeight="11385" xr2:uid="{470C459F-9058-417E-8659-1849A433C267}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -486,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98C40D39-3B0C-4A34-9D0A-C9CE86ABC9FF}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>